<commit_message>
add annex A controls to SoA
</commit_message>
<xml_diff>
--- a/tools/iso27001/iso27001-2022.xlsx
+++ b/tools/iso27001/iso27001-2022.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ericlaubacher/Documents/GitHub/ciso-assistant-community/tools/iso27001/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC2C2B35-0803-E743-A117-48D379C5DD36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A63F4E44-12DF-8F43-90EC-5827ECD67364}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-67840" yWindow="-28300" windowWidth="102400" windowHeight="26600" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="library_content" sheetId="3" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1581" uniqueCount="725">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1674" uniqueCount="818">
   <si>
     <t>library_urn</t>
   </si>
@@ -2215,13 +2215,292 @@
   </si>
   <si>
     <t>Ce document est un résumé de la norme ISO27001-2022. Vous pouvez acheter le standard complet sur https://www.iso.org/standard/27001</t>
+  </si>
+  <si>
+    <t>1:A.5.1</t>
+  </si>
+  <si>
+    <t>1:A.5.2</t>
+  </si>
+  <si>
+    <t>1:A.5.3</t>
+  </si>
+  <si>
+    <t>1:A.5.4</t>
+  </si>
+  <si>
+    <t>1:A.5.5</t>
+  </si>
+  <si>
+    <t>1:A.5.6</t>
+  </si>
+  <si>
+    <t>1:A.5.7</t>
+  </si>
+  <si>
+    <t>1:A.5.8</t>
+  </si>
+  <si>
+    <t>1:A.5.9</t>
+  </si>
+  <si>
+    <t>1:A.5.10</t>
+  </si>
+  <si>
+    <t>1:A.5.11</t>
+  </si>
+  <si>
+    <t>1:A.5.12</t>
+  </si>
+  <si>
+    <t>1:A.5.13</t>
+  </si>
+  <si>
+    <t>1:A.5.14</t>
+  </si>
+  <si>
+    <t>1:A.5.15</t>
+  </si>
+  <si>
+    <t>1:A.5.16</t>
+  </si>
+  <si>
+    <t>1:A.5.17</t>
+  </si>
+  <si>
+    <t>1:A.5.18</t>
+  </si>
+  <si>
+    <t>1:A.5.19</t>
+  </si>
+  <si>
+    <t>1:A.5.20</t>
+  </si>
+  <si>
+    <t>1:A.5.21</t>
+  </si>
+  <si>
+    <t>1:A.5.22</t>
+  </si>
+  <si>
+    <t>1:A.5.23</t>
+  </si>
+  <si>
+    <t>1:A.5.24</t>
+  </si>
+  <si>
+    <t>1:A.5.25</t>
+  </si>
+  <si>
+    <t>1:A.5.26</t>
+  </si>
+  <si>
+    <t>1:A.5.27</t>
+  </si>
+  <si>
+    <t>1:A.5.28</t>
+  </si>
+  <si>
+    <t>1:A.5.29</t>
+  </si>
+  <si>
+    <t>1:A.5.30</t>
+  </si>
+  <si>
+    <t>1:A.5.31</t>
+  </si>
+  <si>
+    <t>1:A.5.32</t>
+  </si>
+  <si>
+    <t>1:A.5.33</t>
+  </si>
+  <si>
+    <t>1:A.5.34</t>
+  </si>
+  <si>
+    <t>1:A.5.35</t>
+  </si>
+  <si>
+    <t>1:A.5.36</t>
+  </si>
+  <si>
+    <t>1:A.5.37</t>
+  </si>
+  <si>
+    <t>1:A.6.1</t>
+  </si>
+  <si>
+    <t>1:A.6.2</t>
+  </si>
+  <si>
+    <t>1:A.6.3</t>
+  </si>
+  <si>
+    <t>1:A.6.4</t>
+  </si>
+  <si>
+    <t>1:A.6.5</t>
+  </si>
+  <si>
+    <t>1:A.6.6</t>
+  </si>
+  <si>
+    <t>1:A.6.7</t>
+  </si>
+  <si>
+    <t>1:A.6.8</t>
+  </si>
+  <si>
+    <t>1:A.7.1</t>
+  </si>
+  <si>
+    <t>1:A.7.2</t>
+  </si>
+  <si>
+    <t>1:A.7.3</t>
+  </si>
+  <si>
+    <t>1:A.7.4</t>
+  </si>
+  <si>
+    <t>1:A.7.5</t>
+  </si>
+  <si>
+    <t>1:A.7.6</t>
+  </si>
+  <si>
+    <t>1:A.7.7</t>
+  </si>
+  <si>
+    <t>1:A.7.8</t>
+  </si>
+  <si>
+    <t>1:A.7.9</t>
+  </si>
+  <si>
+    <t>1:A.7.10</t>
+  </si>
+  <si>
+    <t>1:A.7.11</t>
+  </si>
+  <si>
+    <t>1:A.7.12</t>
+  </si>
+  <si>
+    <t>1:A.7.13</t>
+  </si>
+  <si>
+    <t>1:A.7.14</t>
+  </si>
+  <si>
+    <t>1:A.8.1</t>
+  </si>
+  <si>
+    <t>1:A.8.2</t>
+  </si>
+  <si>
+    <t>1:A.8.3</t>
+  </si>
+  <si>
+    <t>1:A.8.4</t>
+  </si>
+  <si>
+    <t>1:A.8.5</t>
+  </si>
+  <si>
+    <t>1:A.8.6</t>
+  </si>
+  <si>
+    <t>1:A.8.7</t>
+  </si>
+  <si>
+    <t>1:A.8.8</t>
+  </si>
+  <si>
+    <t>1:A.8.9</t>
+  </si>
+  <si>
+    <t>1:A.8.10</t>
+  </si>
+  <si>
+    <t>1:A.8.11</t>
+  </si>
+  <si>
+    <t>1:A.8.12</t>
+  </si>
+  <si>
+    <t>1:A.8.13</t>
+  </si>
+  <si>
+    <t>1:A.8.14</t>
+  </si>
+  <si>
+    <t>1:A.8.15</t>
+  </si>
+  <si>
+    <t>1:A.8.16</t>
+  </si>
+  <si>
+    <t>1:A.8.17</t>
+  </si>
+  <si>
+    <t>1:A.8.18</t>
+  </si>
+  <si>
+    <t>1:A.8.19</t>
+  </si>
+  <si>
+    <t>1:A.8.20</t>
+  </si>
+  <si>
+    <t>1:A.8.21</t>
+  </si>
+  <si>
+    <t>1:A.8.22</t>
+  </si>
+  <si>
+    <t>1:A.8.23</t>
+  </si>
+  <si>
+    <t>1:A.8.24</t>
+  </si>
+  <si>
+    <t>1:A.8.25</t>
+  </si>
+  <si>
+    <t>1:A.8.26</t>
+  </si>
+  <si>
+    <t>1:A.8.27</t>
+  </si>
+  <si>
+    <t>1:A.8.28</t>
+  </si>
+  <si>
+    <t>1:A.8.29</t>
+  </si>
+  <si>
+    <t>1:A.8.30</t>
+  </si>
+  <si>
+    <t>1:A.8.31</t>
+  </si>
+  <si>
+    <t>1:A.8.32</t>
+  </si>
+  <si>
+    <t>1:A.8.33</t>
+  </si>
+  <si>
+    <t>1:A.8.34</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2248,6 +2527,12 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -2643,8 +2928,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61B26082-4BCE-3241-A6CE-5878E545CE62}">
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="166" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView zoomScale="189" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16:XFD16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2667,7 +2952,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -2934,8 +3219,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I144"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="I122" sqref="I122"/>
+    <sheetView tabSelected="1" topLeftCell="A128" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="C141" sqref="C141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3750,7 +4035,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" ht="68" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>295</v>
       </c>
@@ -4146,6 +4431,9 @@
       <c r="F46" s="4" t="s">
         <v>648</v>
       </c>
+      <c r="G46" s="2" t="s">
+        <v>725</v>
+      </c>
       <c r="H46" t="s">
         <v>358</v>
       </c>
@@ -4172,6 +4460,9 @@
       <c r="F47" s="4" t="s">
         <v>649</v>
       </c>
+      <c r="G47" s="2" t="s">
+        <v>726</v>
+      </c>
       <c r="H47" t="s">
         <v>359</v>
       </c>
@@ -4198,6 +4489,9 @@
       <c r="F48" s="4" t="s">
         <v>650</v>
       </c>
+      <c r="G48" s="2" t="s">
+        <v>727</v>
+      </c>
       <c r="H48" t="s">
         <v>360</v>
       </c>
@@ -4224,6 +4518,9 @@
       <c r="F49" s="4" t="s">
         <v>651</v>
       </c>
+      <c r="G49" s="2" t="s">
+        <v>728</v>
+      </c>
       <c r="H49" t="s">
         <v>361</v>
       </c>
@@ -4250,6 +4547,9 @@
       <c r="F50" s="4" t="s">
         <v>652</v>
       </c>
+      <c r="G50" s="2" t="s">
+        <v>729</v>
+      </c>
       <c r="H50" t="s">
         <v>362</v>
       </c>
@@ -4276,6 +4576,9 @@
       <c r="F51" s="4" t="s">
         <v>653</v>
       </c>
+      <c r="G51" s="2" t="s">
+        <v>730</v>
+      </c>
       <c r="H51" t="s">
         <v>363</v>
       </c>
@@ -4302,6 +4605,9 @@
       <c r="F52" s="4" t="s">
         <v>654</v>
       </c>
+      <c r="G52" s="2" t="s">
+        <v>731</v>
+      </c>
       <c r="H52" t="s">
         <v>364</v>
       </c>
@@ -4328,6 +4634,9 @@
       <c r="F53" s="4" t="s">
         <v>655</v>
       </c>
+      <c r="G53" s="2" t="s">
+        <v>732</v>
+      </c>
       <c r="H53" t="s">
         <v>365</v>
       </c>
@@ -4354,6 +4663,9 @@
       <c r="F54" s="4" t="s">
         <v>656</v>
       </c>
+      <c r="G54" s="2" t="s">
+        <v>733</v>
+      </c>
       <c r="H54" t="s">
         <v>366</v>
       </c>
@@ -4380,6 +4692,9 @@
       <c r="F55" s="4" t="s">
         <v>657</v>
       </c>
+      <c r="G55" s="2" t="s">
+        <v>734</v>
+      </c>
       <c r="H55" t="s">
         <v>367</v>
       </c>
@@ -4406,6 +4721,9 @@
       <c r="F56" s="4" t="s">
         <v>658</v>
       </c>
+      <c r="G56" s="2" t="s">
+        <v>735</v>
+      </c>
       <c r="H56" t="s">
         <v>368</v>
       </c>
@@ -4432,6 +4750,9 @@
       <c r="F57" s="4" t="s">
         <v>659</v>
       </c>
+      <c r="G57" s="2" t="s">
+        <v>736</v>
+      </c>
       <c r="H57" t="s">
         <v>369</v>
       </c>
@@ -4458,6 +4779,9 @@
       <c r="F58" s="4" t="s">
         <v>660</v>
       </c>
+      <c r="G58" s="2" t="s">
+        <v>737</v>
+      </c>
       <c r="H58" t="s">
         <v>370</v>
       </c>
@@ -4484,6 +4808,9 @@
       <c r="F59" s="4" t="s">
         <v>661</v>
       </c>
+      <c r="G59" s="2" t="s">
+        <v>738</v>
+      </c>
       <c r="H59" t="s">
         <v>371</v>
       </c>
@@ -4510,6 +4837,9 @@
       <c r="F60" s="4" t="s">
         <v>662</v>
       </c>
+      <c r="G60" s="2" t="s">
+        <v>739</v>
+      </c>
       <c r="H60" t="s">
         <v>372</v>
       </c>
@@ -4536,6 +4866,9 @@
       <c r="F61" s="4" t="s">
         <v>663</v>
       </c>
+      <c r="G61" s="2" t="s">
+        <v>740</v>
+      </c>
       <c r="H61" t="s">
         <v>373</v>
       </c>
@@ -4562,6 +4895,9 @@
       <c r="F62" s="4" t="s">
         <v>664</v>
       </c>
+      <c r="G62" s="2" t="s">
+        <v>741</v>
+      </c>
       <c r="H62" t="s">
         <v>374</v>
       </c>
@@ -4588,6 +4924,9 @@
       <c r="F63" s="4" t="s">
         <v>665</v>
       </c>
+      <c r="G63" s="2" t="s">
+        <v>742</v>
+      </c>
       <c r="H63" t="s">
         <v>375</v>
       </c>
@@ -4614,6 +4953,9 @@
       <c r="F64" s="4" t="s">
         <v>666</v>
       </c>
+      <c r="G64" s="2" t="s">
+        <v>743</v>
+      </c>
       <c r="H64" t="s">
         <v>376</v>
       </c>
@@ -4640,6 +4982,9 @@
       <c r="F65" s="4" t="s">
         <v>667</v>
       </c>
+      <c r="G65" s="2" t="s">
+        <v>744</v>
+      </c>
       <c r="H65" t="s">
         <v>377</v>
       </c>
@@ -4666,6 +5011,9 @@
       <c r="F66" s="4" t="s">
         <v>668</v>
       </c>
+      <c r="G66" s="2" t="s">
+        <v>745</v>
+      </c>
       <c r="H66" t="s">
         <v>378</v>
       </c>
@@ -4692,6 +5040,9 @@
       <c r="F67" s="4" t="s">
         <v>669</v>
       </c>
+      <c r="G67" s="2" t="s">
+        <v>746</v>
+      </c>
       <c r="H67" t="s">
         <v>379</v>
       </c>
@@ -4718,6 +5069,9 @@
       <c r="F68" s="4" t="s">
         <v>670</v>
       </c>
+      <c r="G68" s="2" t="s">
+        <v>747</v>
+      </c>
       <c r="H68" t="s">
         <v>380</v>
       </c>
@@ -4744,6 +5098,9 @@
       <c r="F69" s="4" t="s">
         <v>671</v>
       </c>
+      <c r="G69" s="2" t="s">
+        <v>748</v>
+      </c>
       <c r="H69" t="s">
         <v>381</v>
       </c>
@@ -4751,7 +5108,7 @@
         <v>708</v>
       </c>
     </row>
-    <row r="70" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:9" ht="68" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
         <v>295</v>
       </c>
@@ -4770,6 +5127,9 @@
       <c r="F70" s="4" t="s">
         <v>672</v>
       </c>
+      <c r="G70" s="2" t="s">
+        <v>749</v>
+      </c>
       <c r="H70" t="s">
         <v>382</v>
       </c>
@@ -4796,6 +5156,9 @@
       <c r="F71" s="4" t="s">
         <v>673</v>
       </c>
+      <c r="G71" s="2" t="s">
+        <v>750</v>
+      </c>
       <c r="H71" t="s">
         <v>383</v>
       </c>
@@ -4822,6 +5185,9 @@
       <c r="F72" s="4" t="s">
         <v>674</v>
       </c>
+      <c r="G72" s="2" t="s">
+        <v>751</v>
+      </c>
       <c r="H72" t="s">
         <v>384</v>
       </c>
@@ -4848,6 +5214,9 @@
       <c r="F73" s="4" t="s">
         <v>675</v>
       </c>
+      <c r="G73" s="2" t="s">
+        <v>752</v>
+      </c>
       <c r="H73" t="s">
         <v>385</v>
       </c>
@@ -4874,6 +5243,9 @@
       <c r="F74" s="4" t="s">
         <v>676</v>
       </c>
+      <c r="G74" s="2" t="s">
+        <v>753</v>
+      </c>
       <c r="H74" t="s">
         <v>386</v>
       </c>
@@ -4900,6 +5272,9 @@
       <c r="F75" s="4" t="s">
         <v>677</v>
       </c>
+      <c r="G75" s="2" t="s">
+        <v>754</v>
+      </c>
       <c r="H75" t="s">
         <v>387</v>
       </c>
@@ -4926,6 +5301,9 @@
       <c r="F76" s="4" t="s">
         <v>678</v>
       </c>
+      <c r="G76" s="2" t="s">
+        <v>755</v>
+      </c>
       <c r="H76" t="s">
         <v>388</v>
       </c>
@@ -4952,6 +5330,9 @@
       <c r="F77" s="4" t="s">
         <v>679</v>
       </c>
+      <c r="G77" s="2" t="s">
+        <v>756</v>
+      </c>
       <c r="H77" t="s">
         <v>389</v>
       </c>
@@ -4978,6 +5359,9 @@
       <c r="F78" s="4" t="s">
         <v>680</v>
       </c>
+      <c r="G78" s="2" t="s">
+        <v>757</v>
+      </c>
       <c r="H78" t="s">
         <v>390</v>
       </c>
@@ -5004,6 +5388,9 @@
       <c r="F79" s="4" t="s">
         <v>681</v>
       </c>
+      <c r="G79" s="2" t="s">
+        <v>758</v>
+      </c>
       <c r="H79" t="s">
         <v>391</v>
       </c>
@@ -5030,6 +5417,9 @@
       <c r="F80" s="4" t="s">
         <v>682</v>
       </c>
+      <c r="G80" s="2" t="s">
+        <v>759</v>
+      </c>
       <c r="H80" t="s">
         <v>392</v>
       </c>
@@ -5056,6 +5446,9 @@
       <c r="F81" s="4" t="s">
         <v>683</v>
       </c>
+      <c r="G81" s="2" t="s">
+        <v>760</v>
+      </c>
       <c r="H81" t="s">
         <v>393</v>
       </c>
@@ -5081,6 +5474,9 @@
       </c>
       <c r="F82" s="4" t="s">
         <v>684</v>
+      </c>
+      <c r="G82" s="2" t="s">
+        <v>761</v>
       </c>
       <c r="H82" t="s">
         <v>394</v>
@@ -5108,7 +5504,7 @@
       </c>
       <c r="I83" s="2"/>
     </row>
-    <row r="84" spans="1:9" ht="68" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:9" ht="85" x14ac:dyDescent="0.2">
       <c r="A84" s="2" t="s">
         <v>295</v>
       </c>
@@ -5127,6 +5523,9 @@
       <c r="F84" s="4" t="s">
         <v>632</v>
       </c>
+      <c r="G84" s="2" t="s">
+        <v>762</v>
+      </c>
       <c r="H84" t="s">
         <v>396</v>
       </c>
@@ -5153,6 +5552,9 @@
       <c r="F85" s="4" t="s">
         <v>633</v>
       </c>
+      <c r="G85" s="2" t="s">
+        <v>763</v>
+      </c>
       <c r="H85" t="s">
         <v>397</v>
       </c>
@@ -5179,6 +5581,9 @@
       <c r="F86" s="4" t="s">
         <v>634</v>
       </c>
+      <c r="G86" s="2" t="s">
+        <v>764</v>
+      </c>
       <c r="H86" t="s">
         <v>398</v>
       </c>
@@ -5205,6 +5610,9 @@
       <c r="F87" s="4" t="s">
         <v>635</v>
       </c>
+      <c r="G87" s="2" t="s">
+        <v>765</v>
+      </c>
       <c r="H87" t="s">
         <v>399</v>
       </c>
@@ -5231,6 +5639,9 @@
       <c r="F88" s="4" t="s">
         <v>636</v>
       </c>
+      <c r="G88" s="2" t="s">
+        <v>766</v>
+      </c>
       <c r="H88" t="s">
         <v>400</v>
       </c>
@@ -5257,6 +5668,9 @@
       <c r="F89" s="4" t="s">
         <v>637</v>
       </c>
+      <c r="G89" s="2" t="s">
+        <v>767</v>
+      </c>
       <c r="H89" t="s">
         <v>401</v>
       </c>
@@ -5283,6 +5697,9 @@
       <c r="F90" s="4" t="s">
         <v>638</v>
       </c>
+      <c r="G90" s="2" t="s">
+        <v>768</v>
+      </c>
       <c r="H90" t="s">
         <v>402</v>
       </c>
@@ -5308,6 +5725,9 @@
       </c>
       <c r="F91" s="4" t="s">
         <v>639</v>
+      </c>
+      <c r="G91" s="2" t="s">
+        <v>769</v>
       </c>
       <c r="H91" t="s">
         <v>403</v>
@@ -5354,6 +5774,9 @@
       <c r="F93" s="4" t="s">
         <v>604</v>
       </c>
+      <c r="G93" s="2" t="s">
+        <v>770</v>
+      </c>
       <c r="H93" t="s">
         <v>405</v>
       </c>
@@ -5380,6 +5803,9 @@
       <c r="F94" s="4" t="s">
         <v>605</v>
       </c>
+      <c r="G94" s="2" t="s">
+        <v>771</v>
+      </c>
       <c r="H94" t="s">
         <v>406</v>
       </c>
@@ -5406,6 +5832,9 @@
       <c r="F95" s="4" t="s">
         <v>606</v>
       </c>
+      <c r="G95" s="2" t="s">
+        <v>772</v>
+      </c>
       <c r="H95" t="s">
         <v>407</v>
       </c>
@@ -5432,6 +5861,9 @@
       <c r="F96" s="4" t="s">
         <v>607</v>
       </c>
+      <c r="G96" s="2" t="s">
+        <v>773</v>
+      </c>
       <c r="H96" t="s">
         <v>408</v>
       </c>
@@ -5458,6 +5890,9 @@
       <c r="F97" s="4" t="s">
         <v>608</v>
       </c>
+      <c r="G97" s="2" t="s">
+        <v>774</v>
+      </c>
       <c r="H97" t="s">
         <v>409</v>
       </c>
@@ -5484,6 +5919,9 @@
       <c r="F98" s="4" t="s">
         <v>609</v>
       </c>
+      <c r="G98" s="2" t="s">
+        <v>775</v>
+      </c>
       <c r="H98" t="s">
         <v>410</v>
       </c>
@@ -5510,6 +5948,9 @@
       <c r="F99" s="4" t="s">
         <v>610</v>
       </c>
+      <c r="G99" s="2" t="s">
+        <v>776</v>
+      </c>
       <c r="H99" t="s">
         <v>411</v>
       </c>
@@ -5517,7 +5958,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="100" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:9" ht="68" x14ac:dyDescent="0.2">
       <c r="A100" s="2" t="s">
         <v>295</v>
       </c>
@@ -5536,6 +5977,9 @@
       <c r="F100" s="4" t="s">
         <v>611</v>
       </c>
+      <c r="G100" s="2" t="s">
+        <v>777</v>
+      </c>
       <c r="H100" t="s">
         <v>412</v>
       </c>
@@ -5562,6 +6006,9 @@
       <c r="F101" s="4" t="s">
         <v>612</v>
       </c>
+      <c r="G101" s="2" t="s">
+        <v>778</v>
+      </c>
       <c r="H101" t="s">
         <v>413</v>
       </c>
@@ -5588,6 +6035,9 @@
       <c r="F102" s="4" t="s">
         <v>613</v>
       </c>
+      <c r="G102" s="2" t="s">
+        <v>779</v>
+      </c>
       <c r="H102" t="s">
         <v>414</v>
       </c>
@@ -5595,7 +6045,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="103" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:9" ht="68" x14ac:dyDescent="0.2">
       <c r="A103" s="2" t="s">
         <v>295</v>
       </c>
@@ -5614,6 +6064,9 @@
       <c r="F103" s="4" t="s">
         <v>614</v>
       </c>
+      <c r="G103" s="2" t="s">
+        <v>780</v>
+      </c>
       <c r="H103" t="s">
         <v>415</v>
       </c>
@@ -5640,6 +6093,9 @@
       <c r="F104" s="4" t="s">
         <v>615</v>
       </c>
+      <c r="G104" s="2" t="s">
+        <v>781</v>
+      </c>
       <c r="H104" t="s">
         <v>416</v>
       </c>
@@ -5666,6 +6122,9 @@
       <c r="F105" s="4" t="s">
         <v>616</v>
       </c>
+      <c r="G105" s="2" t="s">
+        <v>782</v>
+      </c>
       <c r="H105" t="s">
         <v>417</v>
       </c>
@@ -5691,6 +6150,9 @@
       </c>
       <c r="F106" s="4" t="s">
         <v>617</v>
+      </c>
+      <c r="G106" s="2" t="s">
+        <v>783</v>
       </c>
       <c r="H106" t="s">
         <v>418</v>
@@ -5737,6 +6199,9 @@
       <c r="F108" s="4" t="s">
         <v>537</v>
       </c>
+      <c r="G108" s="2" t="s">
+        <v>784</v>
+      </c>
       <c r="H108" t="s">
         <v>420</v>
       </c>
@@ -5763,6 +6228,9 @@
       <c r="F109" s="4" t="s">
         <v>538</v>
       </c>
+      <c r="G109" s="2" t="s">
+        <v>785</v>
+      </c>
       <c r="H109" t="s">
         <v>421</v>
       </c>
@@ -5789,6 +6257,9 @@
       <c r="F110" s="4" t="s">
         <v>539</v>
       </c>
+      <c r="G110" s="2" t="s">
+        <v>786</v>
+      </c>
       <c r="H110" t="s">
         <v>422</v>
       </c>
@@ -5815,6 +6286,9 @@
       <c r="F111" s="4" t="s">
         <v>540</v>
       </c>
+      <c r="G111" s="2" t="s">
+        <v>787</v>
+      </c>
       <c r="H111" t="s">
         <v>423</v>
       </c>
@@ -5841,6 +6315,9 @@
       <c r="F112" s="4" t="s">
         <v>541</v>
       </c>
+      <c r="G112" s="2" t="s">
+        <v>788</v>
+      </c>
       <c r="H112" t="s">
         <v>424</v>
       </c>
@@ -5867,6 +6344,9 @@
       <c r="F113" s="4" t="s">
         <v>542</v>
       </c>
+      <c r="G113" s="2" t="s">
+        <v>789</v>
+      </c>
       <c r="H113" t="s">
         <v>425</v>
       </c>
@@ -5893,6 +6373,9 @@
       <c r="F114" s="4" t="s">
         <v>543</v>
       </c>
+      <c r="G114" s="2" t="s">
+        <v>790</v>
+      </c>
       <c r="H114" t="s">
         <v>426</v>
       </c>
@@ -5919,6 +6402,9 @@
       <c r="F115" s="4" t="s">
         <v>544</v>
       </c>
+      <c r="G115" s="2" t="s">
+        <v>791</v>
+      </c>
       <c r="H115" t="s">
         <v>427</v>
       </c>
@@ -5945,6 +6431,9 @@
       <c r="F116" s="4" t="s">
         <v>545</v>
       </c>
+      <c r="G116" s="2" t="s">
+        <v>792</v>
+      </c>
       <c r="H116" t="s">
         <v>428</v>
       </c>
@@ -5971,6 +6460,9 @@
       <c r="F117" s="4" t="s">
         <v>546</v>
       </c>
+      <c r="G117" s="2" t="s">
+        <v>793</v>
+      </c>
       <c r="H117" t="s">
         <v>429</v>
       </c>
@@ -5997,6 +6489,9 @@
       <c r="F118" s="4" t="s">
         <v>547</v>
       </c>
+      <c r="G118" s="2" t="s">
+        <v>794</v>
+      </c>
       <c r="H118" t="s">
         <v>430</v>
       </c>
@@ -6023,6 +6518,9 @@
       <c r="F119" s="4" t="s">
         <v>548</v>
       </c>
+      <c r="G119" s="2" t="s">
+        <v>795</v>
+      </c>
       <c r="H119" t="s">
         <v>431</v>
       </c>
@@ -6049,6 +6547,9 @@
       <c r="F120" s="4" t="s">
         <v>549</v>
       </c>
+      <c r="G120" s="2" t="s">
+        <v>796</v>
+      </c>
       <c r="H120" t="s">
         <v>432</v>
       </c>
@@ -6075,6 +6576,9 @@
       <c r="F121" s="4" t="s">
         <v>550</v>
       </c>
+      <c r="G121" s="2" t="s">
+        <v>797</v>
+      </c>
       <c r="H121" t="s">
         <v>433</v>
       </c>
@@ -6101,6 +6605,9 @@
       <c r="F122" s="4" t="s">
         <v>551</v>
       </c>
+      <c r="G122" s="2" t="s">
+        <v>798</v>
+      </c>
       <c r="H122" t="s">
         <v>434</v>
       </c>
@@ -6127,6 +6634,9 @@
       <c r="F123" s="4" t="s">
         <v>552</v>
       </c>
+      <c r="G123" s="2" t="s">
+        <v>799</v>
+      </c>
       <c r="H123" t="s">
         <v>435</v>
       </c>
@@ -6153,6 +6663,9 @@
       <c r="F124" s="4" t="s">
         <v>553</v>
       </c>
+      <c r="G124" s="2" t="s">
+        <v>800</v>
+      </c>
       <c r="H124" t="s">
         <v>436</v>
       </c>
@@ -6179,6 +6692,9 @@
       <c r="F125" s="4" t="s">
         <v>554</v>
       </c>
+      <c r="G125" s="2" t="s">
+        <v>801</v>
+      </c>
       <c r="H125" t="s">
         <v>437</v>
       </c>
@@ -6205,6 +6721,9 @@
       <c r="F126" s="4" t="s">
         <v>555</v>
       </c>
+      <c r="G126" s="2" t="s">
+        <v>802</v>
+      </c>
       <c r="H126" t="s">
         <v>438</v>
       </c>
@@ -6231,6 +6750,9 @@
       <c r="F127" s="4" t="s">
         <v>556</v>
       </c>
+      <c r="G127" s="2" t="s">
+        <v>803</v>
+      </c>
       <c r="H127" t="s">
         <v>439</v>
       </c>
@@ -6257,6 +6779,9 @@
       <c r="F128" s="4" t="s">
         <v>557</v>
       </c>
+      <c r="G128" s="2" t="s">
+        <v>804</v>
+      </c>
       <c r="H128" t="s">
         <v>440</v>
       </c>
@@ -6283,6 +6808,9 @@
       <c r="F129" s="4" t="s">
         <v>558</v>
       </c>
+      <c r="G129" s="2" t="s">
+        <v>805</v>
+      </c>
       <c r="H129" t="s">
         <v>441</v>
       </c>
@@ -6309,6 +6837,9 @@
       <c r="F130" s="2" t="s">
         <v>559</v>
       </c>
+      <c r="G130" s="2" t="s">
+        <v>806</v>
+      </c>
       <c r="H130" t="s">
         <v>442</v>
       </c>
@@ -6335,6 +6866,9 @@
       <c r="F131" s="2" t="s">
         <v>560</v>
       </c>
+      <c r="G131" s="2" t="s">
+        <v>807</v>
+      </c>
       <c r="H131" t="s">
         <v>443</v>
       </c>
@@ -6361,6 +6895,9 @@
       <c r="F132" s="2" t="s">
         <v>561</v>
       </c>
+      <c r="G132" s="2" t="s">
+        <v>808</v>
+      </c>
       <c r="H132" t="s">
         <v>444</v>
       </c>
@@ -6387,6 +6924,9 @@
       <c r="F133" s="2" t="s">
         <v>562</v>
       </c>
+      <c r="G133" s="2" t="s">
+        <v>809</v>
+      </c>
       <c r="H133" t="s">
         <v>445</v>
       </c>
@@ -6413,6 +6953,9 @@
       <c r="F134" s="2" t="s">
         <v>563</v>
       </c>
+      <c r="G134" s="2" t="s">
+        <v>810</v>
+      </c>
       <c r="H134" t="s">
         <v>446</v>
       </c>
@@ -6439,6 +6982,9 @@
       <c r="F135" s="2" t="s">
         <v>564</v>
       </c>
+      <c r="G135" s="2" t="s">
+        <v>811</v>
+      </c>
       <c r="H135" t="s">
         <v>447</v>
       </c>
@@ -6465,6 +7011,9 @@
       <c r="F136" s="2" t="s">
         <v>565</v>
       </c>
+      <c r="G136" s="2" t="s">
+        <v>812</v>
+      </c>
       <c r="H136" t="s">
         <v>448</v>
       </c>
@@ -6491,6 +7040,9 @@
       <c r="F137" s="2" t="s">
         <v>566</v>
       </c>
+      <c r="G137" s="2" t="s">
+        <v>813</v>
+      </c>
       <c r="H137" t="s">
         <v>449</v>
       </c>
@@ -6517,6 +7069,9 @@
       <c r="F138" s="2" t="s">
         <v>567</v>
       </c>
+      <c r="G138" s="2" t="s">
+        <v>814</v>
+      </c>
       <c r="H138" t="s">
         <v>450</v>
       </c>
@@ -6543,6 +7098,9 @@
       <c r="F139" s="2" t="s">
         <v>568</v>
       </c>
+      <c r="G139" s="2" t="s">
+        <v>815</v>
+      </c>
       <c r="H139" t="s">
         <v>451</v>
       </c>
@@ -6569,6 +7127,9 @@
       <c r="F140" s="2" t="s">
         <v>569</v>
       </c>
+      <c r="G140" s="2" t="s">
+        <v>816</v>
+      </c>
       <c r="H140" t="s">
         <v>452</v>
       </c>
@@ -6594,6 +7155,9 @@
       </c>
       <c r="F141" s="2" t="s">
         <v>570</v>
+      </c>
+      <c r="G141" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="H141" t="s">
         <v>453</v>
@@ -6615,6 +7179,7 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:I141" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -7201,7 +7766,7 @@
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
     </row>
-    <row r="26" spans="1:9" s="5" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" s="5" customFormat="1" ht="68" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>213</v>
       </c>
@@ -7500,7 +8065,7 @@
       <c r="H38" s="2"/>
       <c r="I38" s="2"/>
     </row>
-    <row r="39" spans="1:9" s="5" customFormat="1" ht="68" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:9" s="5" customFormat="1" ht="85" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>225</v>
       </c>
@@ -7845,7 +8410,7 @@
       <c r="H53" s="2"/>
       <c r="I53" s="2"/>
     </row>
-    <row r="54" spans="1:9" s="5" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:9" s="5" customFormat="1" ht="68" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
         <v>240</v>
       </c>
@@ -7914,7 +8479,7 @@
       <c r="H56" s="2"/>
       <c r="I56" s="2"/>
     </row>
-    <row r="57" spans="1:9" s="5" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:9" s="5" customFormat="1" ht="68" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
         <v>243</v>
       </c>

</xml_diff>

<commit_message>
feat(lib): automatically create the controls of SOA on 27001 when requesting suggestions (#1875)
add annex A controls to SoA
</commit_message>
<xml_diff>
--- a/tools/iso27001/iso27001-2022.xlsx
+++ b/tools/iso27001/iso27001-2022.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ericlaubacher/Documents/GitHub/ciso-assistant-community/tools/iso27001/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC2C2B35-0803-E743-A117-48D379C5DD36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A63F4E44-12DF-8F43-90EC-5827ECD67364}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-67840" yWindow="-28300" windowWidth="102400" windowHeight="26600" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="library_content" sheetId="3" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1581" uniqueCount="725">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1674" uniqueCount="818">
   <si>
     <t>library_urn</t>
   </si>
@@ -2215,13 +2215,292 @@
   </si>
   <si>
     <t>Ce document est un résumé de la norme ISO27001-2022. Vous pouvez acheter le standard complet sur https://www.iso.org/standard/27001</t>
+  </si>
+  <si>
+    <t>1:A.5.1</t>
+  </si>
+  <si>
+    <t>1:A.5.2</t>
+  </si>
+  <si>
+    <t>1:A.5.3</t>
+  </si>
+  <si>
+    <t>1:A.5.4</t>
+  </si>
+  <si>
+    <t>1:A.5.5</t>
+  </si>
+  <si>
+    <t>1:A.5.6</t>
+  </si>
+  <si>
+    <t>1:A.5.7</t>
+  </si>
+  <si>
+    <t>1:A.5.8</t>
+  </si>
+  <si>
+    <t>1:A.5.9</t>
+  </si>
+  <si>
+    <t>1:A.5.10</t>
+  </si>
+  <si>
+    <t>1:A.5.11</t>
+  </si>
+  <si>
+    <t>1:A.5.12</t>
+  </si>
+  <si>
+    <t>1:A.5.13</t>
+  </si>
+  <si>
+    <t>1:A.5.14</t>
+  </si>
+  <si>
+    <t>1:A.5.15</t>
+  </si>
+  <si>
+    <t>1:A.5.16</t>
+  </si>
+  <si>
+    <t>1:A.5.17</t>
+  </si>
+  <si>
+    <t>1:A.5.18</t>
+  </si>
+  <si>
+    <t>1:A.5.19</t>
+  </si>
+  <si>
+    <t>1:A.5.20</t>
+  </si>
+  <si>
+    <t>1:A.5.21</t>
+  </si>
+  <si>
+    <t>1:A.5.22</t>
+  </si>
+  <si>
+    <t>1:A.5.23</t>
+  </si>
+  <si>
+    <t>1:A.5.24</t>
+  </si>
+  <si>
+    <t>1:A.5.25</t>
+  </si>
+  <si>
+    <t>1:A.5.26</t>
+  </si>
+  <si>
+    <t>1:A.5.27</t>
+  </si>
+  <si>
+    <t>1:A.5.28</t>
+  </si>
+  <si>
+    <t>1:A.5.29</t>
+  </si>
+  <si>
+    <t>1:A.5.30</t>
+  </si>
+  <si>
+    <t>1:A.5.31</t>
+  </si>
+  <si>
+    <t>1:A.5.32</t>
+  </si>
+  <si>
+    <t>1:A.5.33</t>
+  </si>
+  <si>
+    <t>1:A.5.34</t>
+  </si>
+  <si>
+    <t>1:A.5.35</t>
+  </si>
+  <si>
+    <t>1:A.5.36</t>
+  </si>
+  <si>
+    <t>1:A.5.37</t>
+  </si>
+  <si>
+    <t>1:A.6.1</t>
+  </si>
+  <si>
+    <t>1:A.6.2</t>
+  </si>
+  <si>
+    <t>1:A.6.3</t>
+  </si>
+  <si>
+    <t>1:A.6.4</t>
+  </si>
+  <si>
+    <t>1:A.6.5</t>
+  </si>
+  <si>
+    <t>1:A.6.6</t>
+  </si>
+  <si>
+    <t>1:A.6.7</t>
+  </si>
+  <si>
+    <t>1:A.6.8</t>
+  </si>
+  <si>
+    <t>1:A.7.1</t>
+  </si>
+  <si>
+    <t>1:A.7.2</t>
+  </si>
+  <si>
+    <t>1:A.7.3</t>
+  </si>
+  <si>
+    <t>1:A.7.4</t>
+  </si>
+  <si>
+    <t>1:A.7.5</t>
+  </si>
+  <si>
+    <t>1:A.7.6</t>
+  </si>
+  <si>
+    <t>1:A.7.7</t>
+  </si>
+  <si>
+    <t>1:A.7.8</t>
+  </si>
+  <si>
+    <t>1:A.7.9</t>
+  </si>
+  <si>
+    <t>1:A.7.10</t>
+  </si>
+  <si>
+    <t>1:A.7.11</t>
+  </si>
+  <si>
+    <t>1:A.7.12</t>
+  </si>
+  <si>
+    <t>1:A.7.13</t>
+  </si>
+  <si>
+    <t>1:A.7.14</t>
+  </si>
+  <si>
+    <t>1:A.8.1</t>
+  </si>
+  <si>
+    <t>1:A.8.2</t>
+  </si>
+  <si>
+    <t>1:A.8.3</t>
+  </si>
+  <si>
+    <t>1:A.8.4</t>
+  </si>
+  <si>
+    <t>1:A.8.5</t>
+  </si>
+  <si>
+    <t>1:A.8.6</t>
+  </si>
+  <si>
+    <t>1:A.8.7</t>
+  </si>
+  <si>
+    <t>1:A.8.8</t>
+  </si>
+  <si>
+    <t>1:A.8.9</t>
+  </si>
+  <si>
+    <t>1:A.8.10</t>
+  </si>
+  <si>
+    <t>1:A.8.11</t>
+  </si>
+  <si>
+    <t>1:A.8.12</t>
+  </si>
+  <si>
+    <t>1:A.8.13</t>
+  </si>
+  <si>
+    <t>1:A.8.14</t>
+  </si>
+  <si>
+    <t>1:A.8.15</t>
+  </si>
+  <si>
+    <t>1:A.8.16</t>
+  </si>
+  <si>
+    <t>1:A.8.17</t>
+  </si>
+  <si>
+    <t>1:A.8.18</t>
+  </si>
+  <si>
+    <t>1:A.8.19</t>
+  </si>
+  <si>
+    <t>1:A.8.20</t>
+  </si>
+  <si>
+    <t>1:A.8.21</t>
+  </si>
+  <si>
+    <t>1:A.8.22</t>
+  </si>
+  <si>
+    <t>1:A.8.23</t>
+  </si>
+  <si>
+    <t>1:A.8.24</t>
+  </si>
+  <si>
+    <t>1:A.8.25</t>
+  </si>
+  <si>
+    <t>1:A.8.26</t>
+  </si>
+  <si>
+    <t>1:A.8.27</t>
+  </si>
+  <si>
+    <t>1:A.8.28</t>
+  </si>
+  <si>
+    <t>1:A.8.29</t>
+  </si>
+  <si>
+    <t>1:A.8.30</t>
+  </si>
+  <si>
+    <t>1:A.8.31</t>
+  </si>
+  <si>
+    <t>1:A.8.32</t>
+  </si>
+  <si>
+    <t>1:A.8.33</t>
+  </si>
+  <si>
+    <t>1:A.8.34</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2248,6 +2527,12 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -2643,8 +2928,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61B26082-4BCE-3241-A6CE-5878E545CE62}">
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="166" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView zoomScale="189" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16:XFD16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2667,7 +2952,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -2934,8 +3219,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I144"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="I122" sqref="I122"/>
+    <sheetView tabSelected="1" topLeftCell="A128" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="C141" sqref="C141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3750,7 +4035,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" ht="68" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>295</v>
       </c>
@@ -4146,6 +4431,9 @@
       <c r="F46" s="4" t="s">
         <v>648</v>
       </c>
+      <c r="G46" s="2" t="s">
+        <v>725</v>
+      </c>
       <c r="H46" t="s">
         <v>358</v>
       </c>
@@ -4172,6 +4460,9 @@
       <c r="F47" s="4" t="s">
         <v>649</v>
       </c>
+      <c r="G47" s="2" t="s">
+        <v>726</v>
+      </c>
       <c r="H47" t="s">
         <v>359</v>
       </c>
@@ -4198,6 +4489,9 @@
       <c r="F48" s="4" t="s">
         <v>650</v>
       </c>
+      <c r="G48" s="2" t="s">
+        <v>727</v>
+      </c>
       <c r="H48" t="s">
         <v>360</v>
       </c>
@@ -4224,6 +4518,9 @@
       <c r="F49" s="4" t="s">
         <v>651</v>
       </c>
+      <c r="G49" s="2" t="s">
+        <v>728</v>
+      </c>
       <c r="H49" t="s">
         <v>361</v>
       </c>
@@ -4250,6 +4547,9 @@
       <c r="F50" s="4" t="s">
         <v>652</v>
       </c>
+      <c r="G50" s="2" t="s">
+        <v>729</v>
+      </c>
       <c r="H50" t="s">
         <v>362</v>
       </c>
@@ -4276,6 +4576,9 @@
       <c r="F51" s="4" t="s">
         <v>653</v>
       </c>
+      <c r="G51" s="2" t="s">
+        <v>730</v>
+      </c>
       <c r="H51" t="s">
         <v>363</v>
       </c>
@@ -4302,6 +4605,9 @@
       <c r="F52" s="4" t="s">
         <v>654</v>
       </c>
+      <c r="G52" s="2" t="s">
+        <v>731</v>
+      </c>
       <c r="H52" t="s">
         <v>364</v>
       </c>
@@ -4328,6 +4634,9 @@
       <c r="F53" s="4" t="s">
         <v>655</v>
       </c>
+      <c r="G53" s="2" t="s">
+        <v>732</v>
+      </c>
       <c r="H53" t="s">
         <v>365</v>
       </c>
@@ -4354,6 +4663,9 @@
       <c r="F54" s="4" t="s">
         <v>656</v>
       </c>
+      <c r="G54" s="2" t="s">
+        <v>733</v>
+      </c>
       <c r="H54" t="s">
         <v>366</v>
       </c>
@@ -4380,6 +4692,9 @@
       <c r="F55" s="4" t="s">
         <v>657</v>
       </c>
+      <c r="G55" s="2" t="s">
+        <v>734</v>
+      </c>
       <c r="H55" t="s">
         <v>367</v>
       </c>
@@ -4406,6 +4721,9 @@
       <c r="F56" s="4" t="s">
         <v>658</v>
       </c>
+      <c r="G56" s="2" t="s">
+        <v>735</v>
+      </c>
       <c r="H56" t="s">
         <v>368</v>
       </c>
@@ -4432,6 +4750,9 @@
       <c r="F57" s="4" t="s">
         <v>659</v>
       </c>
+      <c r="G57" s="2" t="s">
+        <v>736</v>
+      </c>
       <c r="H57" t="s">
         <v>369</v>
       </c>
@@ -4458,6 +4779,9 @@
       <c r="F58" s="4" t="s">
         <v>660</v>
       </c>
+      <c r="G58" s="2" t="s">
+        <v>737</v>
+      </c>
       <c r="H58" t="s">
         <v>370</v>
       </c>
@@ -4484,6 +4808,9 @@
       <c r="F59" s="4" t="s">
         <v>661</v>
       </c>
+      <c r="G59" s="2" t="s">
+        <v>738</v>
+      </c>
       <c r="H59" t="s">
         <v>371</v>
       </c>
@@ -4510,6 +4837,9 @@
       <c r="F60" s="4" t="s">
         <v>662</v>
       </c>
+      <c r="G60" s="2" t="s">
+        <v>739</v>
+      </c>
       <c r="H60" t="s">
         <v>372</v>
       </c>
@@ -4536,6 +4866,9 @@
       <c r="F61" s="4" t="s">
         <v>663</v>
       </c>
+      <c r="G61" s="2" t="s">
+        <v>740</v>
+      </c>
       <c r="H61" t="s">
         <v>373</v>
       </c>
@@ -4562,6 +4895,9 @@
       <c r="F62" s="4" t="s">
         <v>664</v>
       </c>
+      <c r="G62" s="2" t="s">
+        <v>741</v>
+      </c>
       <c r="H62" t="s">
         <v>374</v>
       </c>
@@ -4588,6 +4924,9 @@
       <c r="F63" s="4" t="s">
         <v>665</v>
       </c>
+      <c r="G63" s="2" t="s">
+        <v>742</v>
+      </c>
       <c r="H63" t="s">
         <v>375</v>
       </c>
@@ -4614,6 +4953,9 @@
       <c r="F64" s="4" t="s">
         <v>666</v>
       </c>
+      <c r="G64" s="2" t="s">
+        <v>743</v>
+      </c>
       <c r="H64" t="s">
         <v>376</v>
       </c>
@@ -4640,6 +4982,9 @@
       <c r="F65" s="4" t="s">
         <v>667</v>
       </c>
+      <c r="G65" s="2" t="s">
+        <v>744</v>
+      </c>
       <c r="H65" t="s">
         <v>377</v>
       </c>
@@ -4666,6 +5011,9 @@
       <c r="F66" s="4" t="s">
         <v>668</v>
       </c>
+      <c r="G66" s="2" t="s">
+        <v>745</v>
+      </c>
       <c r="H66" t="s">
         <v>378</v>
       </c>
@@ -4692,6 +5040,9 @@
       <c r="F67" s="4" t="s">
         <v>669</v>
       </c>
+      <c r="G67" s="2" t="s">
+        <v>746</v>
+      </c>
       <c r="H67" t="s">
         <v>379</v>
       </c>
@@ -4718,6 +5069,9 @@
       <c r="F68" s="4" t="s">
         <v>670</v>
       </c>
+      <c r="G68" s="2" t="s">
+        <v>747</v>
+      </c>
       <c r="H68" t="s">
         <v>380</v>
       </c>
@@ -4744,6 +5098,9 @@
       <c r="F69" s="4" t="s">
         <v>671</v>
       </c>
+      <c r="G69" s="2" t="s">
+        <v>748</v>
+      </c>
       <c r="H69" t="s">
         <v>381</v>
       </c>
@@ -4751,7 +5108,7 @@
         <v>708</v>
       </c>
     </row>
-    <row r="70" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:9" ht="68" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
         <v>295</v>
       </c>
@@ -4770,6 +5127,9 @@
       <c r="F70" s="4" t="s">
         <v>672</v>
       </c>
+      <c r="G70" s="2" t="s">
+        <v>749</v>
+      </c>
       <c r="H70" t="s">
         <v>382</v>
       </c>
@@ -4796,6 +5156,9 @@
       <c r="F71" s="4" t="s">
         <v>673</v>
       </c>
+      <c r="G71" s="2" t="s">
+        <v>750</v>
+      </c>
       <c r="H71" t="s">
         <v>383</v>
       </c>
@@ -4822,6 +5185,9 @@
       <c r="F72" s="4" t="s">
         <v>674</v>
       </c>
+      <c r="G72" s="2" t="s">
+        <v>751</v>
+      </c>
       <c r="H72" t="s">
         <v>384</v>
       </c>
@@ -4848,6 +5214,9 @@
       <c r="F73" s="4" t="s">
         <v>675</v>
       </c>
+      <c r="G73" s="2" t="s">
+        <v>752</v>
+      </c>
       <c r="H73" t="s">
         <v>385</v>
       </c>
@@ -4874,6 +5243,9 @@
       <c r="F74" s="4" t="s">
         <v>676</v>
       </c>
+      <c r="G74" s="2" t="s">
+        <v>753</v>
+      </c>
       <c r="H74" t="s">
         <v>386</v>
       </c>
@@ -4900,6 +5272,9 @@
       <c r="F75" s="4" t="s">
         <v>677</v>
       </c>
+      <c r="G75" s="2" t="s">
+        <v>754</v>
+      </c>
       <c r="H75" t="s">
         <v>387</v>
       </c>
@@ -4926,6 +5301,9 @@
       <c r="F76" s="4" t="s">
         <v>678</v>
       </c>
+      <c r="G76" s="2" t="s">
+        <v>755</v>
+      </c>
       <c r="H76" t="s">
         <v>388</v>
       </c>
@@ -4952,6 +5330,9 @@
       <c r="F77" s="4" t="s">
         <v>679</v>
       </c>
+      <c r="G77" s="2" t="s">
+        <v>756</v>
+      </c>
       <c r="H77" t="s">
         <v>389</v>
       </c>
@@ -4978,6 +5359,9 @@
       <c r="F78" s="4" t="s">
         <v>680</v>
       </c>
+      <c r="G78" s="2" t="s">
+        <v>757</v>
+      </c>
       <c r="H78" t="s">
         <v>390</v>
       </c>
@@ -5004,6 +5388,9 @@
       <c r="F79" s="4" t="s">
         <v>681</v>
       </c>
+      <c r="G79" s="2" t="s">
+        <v>758</v>
+      </c>
       <c r="H79" t="s">
         <v>391</v>
       </c>
@@ -5030,6 +5417,9 @@
       <c r="F80" s="4" t="s">
         <v>682</v>
       </c>
+      <c r="G80" s="2" t="s">
+        <v>759</v>
+      </c>
       <c r="H80" t="s">
         <v>392</v>
       </c>
@@ -5056,6 +5446,9 @@
       <c r="F81" s="4" t="s">
         <v>683</v>
       </c>
+      <c r="G81" s="2" t="s">
+        <v>760</v>
+      </c>
       <c r="H81" t="s">
         <v>393</v>
       </c>
@@ -5081,6 +5474,9 @@
       </c>
       <c r="F82" s="4" t="s">
         <v>684</v>
+      </c>
+      <c r="G82" s="2" t="s">
+        <v>761</v>
       </c>
       <c r="H82" t="s">
         <v>394</v>
@@ -5108,7 +5504,7 @@
       </c>
       <c r="I83" s="2"/>
     </row>
-    <row r="84" spans="1:9" ht="68" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:9" ht="85" x14ac:dyDescent="0.2">
       <c r="A84" s="2" t="s">
         <v>295</v>
       </c>
@@ -5127,6 +5523,9 @@
       <c r="F84" s="4" t="s">
         <v>632</v>
       </c>
+      <c r="G84" s="2" t="s">
+        <v>762</v>
+      </c>
       <c r="H84" t="s">
         <v>396</v>
       </c>
@@ -5153,6 +5552,9 @@
       <c r="F85" s="4" t="s">
         <v>633</v>
       </c>
+      <c r="G85" s="2" t="s">
+        <v>763</v>
+      </c>
       <c r="H85" t="s">
         <v>397</v>
       </c>
@@ -5179,6 +5581,9 @@
       <c r="F86" s="4" t="s">
         <v>634</v>
       </c>
+      <c r="G86" s="2" t="s">
+        <v>764</v>
+      </c>
       <c r="H86" t="s">
         <v>398</v>
       </c>
@@ -5205,6 +5610,9 @@
       <c r="F87" s="4" t="s">
         <v>635</v>
       </c>
+      <c r="G87" s="2" t="s">
+        <v>765</v>
+      </c>
       <c r="H87" t="s">
         <v>399</v>
       </c>
@@ -5231,6 +5639,9 @@
       <c r="F88" s="4" t="s">
         <v>636</v>
       </c>
+      <c r="G88" s="2" t="s">
+        <v>766</v>
+      </c>
       <c r="H88" t="s">
         <v>400</v>
       </c>
@@ -5257,6 +5668,9 @@
       <c r="F89" s="4" t="s">
         <v>637</v>
       </c>
+      <c r="G89" s="2" t="s">
+        <v>767</v>
+      </c>
       <c r="H89" t="s">
         <v>401</v>
       </c>
@@ -5283,6 +5697,9 @@
       <c r="F90" s="4" t="s">
         <v>638</v>
       </c>
+      <c r="G90" s="2" t="s">
+        <v>768</v>
+      </c>
       <c r="H90" t="s">
         <v>402</v>
       </c>
@@ -5308,6 +5725,9 @@
       </c>
       <c r="F91" s="4" t="s">
         <v>639</v>
+      </c>
+      <c r="G91" s="2" t="s">
+        <v>769</v>
       </c>
       <c r="H91" t="s">
         <v>403</v>
@@ -5354,6 +5774,9 @@
       <c r="F93" s="4" t="s">
         <v>604</v>
       </c>
+      <c r="G93" s="2" t="s">
+        <v>770</v>
+      </c>
       <c r="H93" t="s">
         <v>405</v>
       </c>
@@ -5380,6 +5803,9 @@
       <c r="F94" s="4" t="s">
         <v>605</v>
       </c>
+      <c r="G94" s="2" t="s">
+        <v>771</v>
+      </c>
       <c r="H94" t="s">
         <v>406</v>
       </c>
@@ -5406,6 +5832,9 @@
       <c r="F95" s="4" t="s">
         <v>606</v>
       </c>
+      <c r="G95" s="2" t="s">
+        <v>772</v>
+      </c>
       <c r="H95" t="s">
         <v>407</v>
       </c>
@@ -5432,6 +5861,9 @@
       <c r="F96" s="4" t="s">
         <v>607</v>
       </c>
+      <c r="G96" s="2" t="s">
+        <v>773</v>
+      </c>
       <c r="H96" t="s">
         <v>408</v>
       </c>
@@ -5458,6 +5890,9 @@
       <c r="F97" s="4" t="s">
         <v>608</v>
       </c>
+      <c r="G97" s="2" t="s">
+        <v>774</v>
+      </c>
       <c r="H97" t="s">
         <v>409</v>
       </c>
@@ -5484,6 +5919,9 @@
       <c r="F98" s="4" t="s">
         <v>609</v>
       </c>
+      <c r="G98" s="2" t="s">
+        <v>775</v>
+      </c>
       <c r="H98" t="s">
         <v>410</v>
       </c>
@@ -5510,6 +5948,9 @@
       <c r="F99" s="4" t="s">
         <v>610</v>
       </c>
+      <c r="G99" s="2" t="s">
+        <v>776</v>
+      </c>
       <c r="H99" t="s">
         <v>411</v>
       </c>
@@ -5517,7 +5958,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="100" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:9" ht="68" x14ac:dyDescent="0.2">
       <c r="A100" s="2" t="s">
         <v>295</v>
       </c>
@@ -5536,6 +5977,9 @@
       <c r="F100" s="4" t="s">
         <v>611</v>
       </c>
+      <c r="G100" s="2" t="s">
+        <v>777</v>
+      </c>
       <c r="H100" t="s">
         <v>412</v>
       </c>
@@ -5562,6 +6006,9 @@
       <c r="F101" s="4" t="s">
         <v>612</v>
       </c>
+      <c r="G101" s="2" t="s">
+        <v>778</v>
+      </c>
       <c r="H101" t="s">
         <v>413</v>
       </c>
@@ -5588,6 +6035,9 @@
       <c r="F102" s="4" t="s">
         <v>613</v>
       </c>
+      <c r="G102" s="2" t="s">
+        <v>779</v>
+      </c>
       <c r="H102" t="s">
         <v>414</v>
       </c>
@@ -5595,7 +6045,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="103" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:9" ht="68" x14ac:dyDescent="0.2">
       <c r="A103" s="2" t="s">
         <v>295</v>
       </c>
@@ -5614,6 +6064,9 @@
       <c r="F103" s="4" t="s">
         <v>614</v>
       </c>
+      <c r="G103" s="2" t="s">
+        <v>780</v>
+      </c>
       <c r="H103" t="s">
         <v>415</v>
       </c>
@@ -5640,6 +6093,9 @@
       <c r="F104" s="4" t="s">
         <v>615</v>
       </c>
+      <c r="G104" s="2" t="s">
+        <v>781</v>
+      </c>
       <c r="H104" t="s">
         <v>416</v>
       </c>
@@ -5666,6 +6122,9 @@
       <c r="F105" s="4" t="s">
         <v>616</v>
       </c>
+      <c r="G105" s="2" t="s">
+        <v>782</v>
+      </c>
       <c r="H105" t="s">
         <v>417</v>
       </c>
@@ -5691,6 +6150,9 @@
       </c>
       <c r="F106" s="4" t="s">
         <v>617</v>
+      </c>
+      <c r="G106" s="2" t="s">
+        <v>783</v>
       </c>
       <c r="H106" t="s">
         <v>418</v>
@@ -5737,6 +6199,9 @@
       <c r="F108" s="4" t="s">
         <v>537</v>
       </c>
+      <c r="G108" s="2" t="s">
+        <v>784</v>
+      </c>
       <c r="H108" t="s">
         <v>420</v>
       </c>
@@ -5763,6 +6228,9 @@
       <c r="F109" s="4" t="s">
         <v>538</v>
       </c>
+      <c r="G109" s="2" t="s">
+        <v>785</v>
+      </c>
       <c r="H109" t="s">
         <v>421</v>
       </c>
@@ -5789,6 +6257,9 @@
       <c r="F110" s="4" t="s">
         <v>539</v>
       </c>
+      <c r="G110" s="2" t="s">
+        <v>786</v>
+      </c>
       <c r="H110" t="s">
         <v>422</v>
       </c>
@@ -5815,6 +6286,9 @@
       <c r="F111" s="4" t="s">
         <v>540</v>
       </c>
+      <c r="G111" s="2" t="s">
+        <v>787</v>
+      </c>
       <c r="H111" t="s">
         <v>423</v>
       </c>
@@ -5841,6 +6315,9 @@
       <c r="F112" s="4" t="s">
         <v>541</v>
       </c>
+      <c r="G112" s="2" t="s">
+        <v>788</v>
+      </c>
       <c r="H112" t="s">
         <v>424</v>
       </c>
@@ -5867,6 +6344,9 @@
       <c r="F113" s="4" t="s">
         <v>542</v>
       </c>
+      <c r="G113" s="2" t="s">
+        <v>789</v>
+      </c>
       <c r="H113" t="s">
         <v>425</v>
       </c>
@@ -5893,6 +6373,9 @@
       <c r="F114" s="4" t="s">
         <v>543</v>
       </c>
+      <c r="G114" s="2" t="s">
+        <v>790</v>
+      </c>
       <c r="H114" t="s">
         <v>426</v>
       </c>
@@ -5919,6 +6402,9 @@
       <c r="F115" s="4" t="s">
         <v>544</v>
       </c>
+      <c r="G115" s="2" t="s">
+        <v>791</v>
+      </c>
       <c r="H115" t="s">
         <v>427</v>
       </c>
@@ -5945,6 +6431,9 @@
       <c r="F116" s="4" t="s">
         <v>545</v>
       </c>
+      <c r="G116" s="2" t="s">
+        <v>792</v>
+      </c>
       <c r="H116" t="s">
         <v>428</v>
       </c>
@@ -5971,6 +6460,9 @@
       <c r="F117" s="4" t="s">
         <v>546</v>
       </c>
+      <c r="G117" s="2" t="s">
+        <v>793</v>
+      </c>
       <c r="H117" t="s">
         <v>429</v>
       </c>
@@ -5997,6 +6489,9 @@
       <c r="F118" s="4" t="s">
         <v>547</v>
       </c>
+      <c r="G118" s="2" t="s">
+        <v>794</v>
+      </c>
       <c r="H118" t="s">
         <v>430</v>
       </c>
@@ -6023,6 +6518,9 @@
       <c r="F119" s="4" t="s">
         <v>548</v>
       </c>
+      <c r="G119" s="2" t="s">
+        <v>795</v>
+      </c>
       <c r="H119" t="s">
         <v>431</v>
       </c>
@@ -6049,6 +6547,9 @@
       <c r="F120" s="4" t="s">
         <v>549</v>
       </c>
+      <c r="G120" s="2" t="s">
+        <v>796</v>
+      </c>
       <c r="H120" t="s">
         <v>432</v>
       </c>
@@ -6075,6 +6576,9 @@
       <c r="F121" s="4" t="s">
         <v>550</v>
       </c>
+      <c r="G121" s="2" t="s">
+        <v>797</v>
+      </c>
       <c r="H121" t="s">
         <v>433</v>
       </c>
@@ -6101,6 +6605,9 @@
       <c r="F122" s="4" t="s">
         <v>551</v>
       </c>
+      <c r="G122" s="2" t="s">
+        <v>798</v>
+      </c>
       <c r="H122" t="s">
         <v>434</v>
       </c>
@@ -6127,6 +6634,9 @@
       <c r="F123" s="4" t="s">
         <v>552</v>
       </c>
+      <c r="G123" s="2" t="s">
+        <v>799</v>
+      </c>
       <c r="H123" t="s">
         <v>435</v>
       </c>
@@ -6153,6 +6663,9 @@
       <c r="F124" s="4" t="s">
         <v>553</v>
       </c>
+      <c r="G124" s="2" t="s">
+        <v>800</v>
+      </c>
       <c r="H124" t="s">
         <v>436</v>
       </c>
@@ -6179,6 +6692,9 @@
       <c r="F125" s="4" t="s">
         <v>554</v>
       </c>
+      <c r="G125" s="2" t="s">
+        <v>801</v>
+      </c>
       <c r="H125" t="s">
         <v>437</v>
       </c>
@@ -6205,6 +6721,9 @@
       <c r="F126" s="4" t="s">
         <v>555</v>
       </c>
+      <c r="G126" s="2" t="s">
+        <v>802</v>
+      </c>
       <c r="H126" t="s">
         <v>438</v>
       </c>
@@ -6231,6 +6750,9 @@
       <c r="F127" s="4" t="s">
         <v>556</v>
       </c>
+      <c r="G127" s="2" t="s">
+        <v>803</v>
+      </c>
       <c r="H127" t="s">
         <v>439</v>
       </c>
@@ -6257,6 +6779,9 @@
       <c r="F128" s="4" t="s">
         <v>557</v>
       </c>
+      <c r="G128" s="2" t="s">
+        <v>804</v>
+      </c>
       <c r="H128" t="s">
         <v>440</v>
       </c>
@@ -6283,6 +6808,9 @@
       <c r="F129" s="4" t="s">
         <v>558</v>
       </c>
+      <c r="G129" s="2" t="s">
+        <v>805</v>
+      </c>
       <c r="H129" t="s">
         <v>441</v>
       </c>
@@ -6309,6 +6837,9 @@
       <c r="F130" s="2" t="s">
         <v>559</v>
       </c>
+      <c r="G130" s="2" t="s">
+        <v>806</v>
+      </c>
       <c r="H130" t="s">
         <v>442</v>
       </c>
@@ -6335,6 +6866,9 @@
       <c r="F131" s="2" t="s">
         <v>560</v>
       </c>
+      <c r="G131" s="2" t="s">
+        <v>807</v>
+      </c>
       <c r="H131" t="s">
         <v>443</v>
       </c>
@@ -6361,6 +6895,9 @@
       <c r="F132" s="2" t="s">
         <v>561</v>
       </c>
+      <c r="G132" s="2" t="s">
+        <v>808</v>
+      </c>
       <c r="H132" t="s">
         <v>444</v>
       </c>
@@ -6387,6 +6924,9 @@
       <c r="F133" s="2" t="s">
         <v>562</v>
       </c>
+      <c r="G133" s="2" t="s">
+        <v>809</v>
+      </c>
       <c r="H133" t="s">
         <v>445</v>
       </c>
@@ -6413,6 +6953,9 @@
       <c r="F134" s="2" t="s">
         <v>563</v>
       </c>
+      <c r="G134" s="2" t="s">
+        <v>810</v>
+      </c>
       <c r="H134" t="s">
         <v>446</v>
       </c>
@@ -6439,6 +6982,9 @@
       <c r="F135" s="2" t="s">
         <v>564</v>
       </c>
+      <c r="G135" s="2" t="s">
+        <v>811</v>
+      </c>
       <c r="H135" t="s">
         <v>447</v>
       </c>
@@ -6465,6 +7011,9 @@
       <c r="F136" s="2" t="s">
         <v>565</v>
       </c>
+      <c r="G136" s="2" t="s">
+        <v>812</v>
+      </c>
       <c r="H136" t="s">
         <v>448</v>
       </c>
@@ -6491,6 +7040,9 @@
       <c r="F137" s="2" t="s">
         <v>566</v>
       </c>
+      <c r="G137" s="2" t="s">
+        <v>813</v>
+      </c>
       <c r="H137" t="s">
         <v>449</v>
       </c>
@@ -6517,6 +7069,9 @@
       <c r="F138" s="2" t="s">
         <v>567</v>
       </c>
+      <c r="G138" s="2" t="s">
+        <v>814</v>
+      </c>
       <c r="H138" t="s">
         <v>450</v>
       </c>
@@ -6543,6 +7098,9 @@
       <c r="F139" s="2" t="s">
         <v>568</v>
       </c>
+      <c r="G139" s="2" t="s">
+        <v>815</v>
+      </c>
       <c r="H139" t="s">
         <v>451</v>
       </c>
@@ -6569,6 +7127,9 @@
       <c r="F140" s="2" t="s">
         <v>569</v>
       </c>
+      <c r="G140" s="2" t="s">
+        <v>816</v>
+      </c>
       <c r="H140" t="s">
         <v>452</v>
       </c>
@@ -6594,6 +7155,9 @@
       </c>
       <c r="F141" s="2" t="s">
         <v>570</v>
+      </c>
+      <c r="G141" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="H141" t="s">
         <v>453</v>
@@ -6615,6 +7179,7 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:I141" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -7201,7 +7766,7 @@
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
     </row>
-    <row r="26" spans="1:9" s="5" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" s="5" customFormat="1" ht="68" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>213</v>
       </c>
@@ -7500,7 +8065,7 @@
       <c r="H38" s="2"/>
       <c r="I38" s="2"/>
     </row>
-    <row r="39" spans="1:9" s="5" customFormat="1" ht="68" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:9" s="5" customFormat="1" ht="85" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>225</v>
       </c>
@@ -7845,7 +8410,7 @@
       <c r="H53" s="2"/>
       <c r="I53" s="2"/>
     </row>
-    <row r="54" spans="1:9" s="5" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:9" s="5" customFormat="1" ht="68" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
         <v>240</v>
       </c>
@@ -7914,7 +8479,7 @@
       <c r="H56" s="2"/>
       <c r="I56" s="2"/>
     </row>
-    <row r="57" spans="1:9" s="5" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:9" s="5" customFormat="1" ht="68" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
         <v>243</v>
       </c>

</xml_diff>